<commit_message>
add rotten tomatoes test cases with spacy
</commit_message>
<xml_diff>
--- a/notebooks_rotten_tomatoes_spacy/test_cases/approach2.xlsx
+++ b/notebooks_rotten_tomatoes_spacy/test_cases/approach2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,73 +436,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>template_index</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>original_text</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>masked_text</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>template_text</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>well before the end , the film grows as dull as its characters , about whose fate it is hard to care .</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>well before the end , the film {mask} as {mask} as its characters , about whose fate it is hard to care .</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>well before the end , the film {neg_verb} as {neg_adj} as its characters , about whose fate it is hard to care .</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>taylor tries to shift the tone to a thriller's rush .</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>taylor {mask} to {mask} the tone to a thriller 's rush .</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>taylor {neg_verb} to {neg_verb} the tone to a thriller 's rush .</t>
         </is>
       </c>
     </row>

</xml_diff>